<commit_message>
images added to first view
</commit_message>
<xml_diff>
--- a/accordion-rental/backend/model.xlsx
+++ b/accordion-rental/backend/model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/cs50/166232074/project2/accordion-rental/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5B1FF0-4DCE-6D4D-9BF1-6E4EFD807F85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43531D59-ADD7-FC43-81C4-C53865F5FA81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="5560" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="3520" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,6 +185,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -541,10 +542,10 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -661,16 +662,16 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>34</v>
+        <v>33.5</v>
       </c>
       <c r="Q2">
-        <v>18</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="R2">
-        <v>6</v>
+        <v>6.2</v>
       </c>
       <c r="S2">
-        <v>37</v>
+        <v>32.5</v>
       </c>
       <c r="T2">
         <v>2900</v>
@@ -814,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>26</v>
@@ -1636,16 +1637,16 @@
         <v>3</v>
       </c>
       <c r="P17">
-        <v>38</v>
+        <v>41.2</v>
       </c>
       <c r="Q17">
-        <v>18</v>
+        <v>19.2</v>
       </c>
       <c r="R17">
-        <v>8</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="S17">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="T17">
         <v>2000</v>
@@ -1766,16 +1767,16 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>34</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="Q19">
-        <v>18</v>
+        <v>18.2</v>
       </c>
       <c r="R19">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="S19">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="T19">
         <v>2500</v>
@@ -1831,16 +1832,16 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <v>36</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="Q20">
-        <v>18</v>
+        <v>18.2</v>
       </c>
       <c r="R20">
-        <v>5</v>
+        <v>5.8</v>
       </c>
       <c r="S20">
-        <v>37</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="T20">
         <v>2000</v>

</xml_diff>